<commit_message>
maven setup with compiler
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/test.xlsx
+++ b/src/test/resources/TestData/test.xlsx
@@ -26,12 +26,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
   <si>
     <t>Links</t>
   </si>
   <si>
     <t>http://localhost:3000/feed</t>
+  </si>
+  <si>
+    <t>https://doctube.com/trending-videos</t>
   </si>
 </sst>
 </file>
@@ -378,7 +381,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>